<commit_message>
added dox file for CC evaluation
</commit_message>
<xml_diff>
--- a/New Language/Syntacticcally replaceable.xlsx
+++ b/New Language/Syntacticcally replaceable.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\omer\myGitHub\Front-End-Compiler-Project\New Language\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects_collab\Front-End-Compiler-Project\New Language\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF2B9E4-72A5-4DAB-BB50-4040A9B5B0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="91">
   <si>
     <t>abstract</t>
   </si>
@@ -276,38 +275,95 @@
     <t>String</t>
   </si>
   <si>
-    <t>ENG</t>
-  </si>
-  <si>
     <t>Three ps</t>
   </si>
   <si>
-    <t>While</t>
-  </si>
-  <si>
-    <t>Loop till</t>
-  </si>
-  <si>
-    <t>For</t>
-  </si>
-  <si>
-    <t>Loop thoru</t>
-  </si>
-  <si>
-    <t>loopTill</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Mio</t>
+  </si>
+  <si>
+    <t>str</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>Class name(inherited class){}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if </t>
+  </si>
+  <si>
+    <t xml:space="preserve">loop till </t>
+  </si>
+  <si>
+    <t xml:space="preserve">do till </t>
+  </si>
+  <si>
+    <t>loop thru</t>
+  </si>
+  <si>
+    <t>shift</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>cont</t>
+  </si>
+  <si>
+    <t>ret</t>
+  </si>
+  <si>
+    <t>point</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>dynamic (int/float)</t>
+  </si>
+  <si>
+    <t>val</t>
+  </si>
+  <si>
+    <t>implicit</t>
+  </si>
+  <si>
+    <t>begin/end</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>Const</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>MiO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,8 +411,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,8 +443,18 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -384,73 +464,58 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -464,42 +529,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="4" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -776,20 +830,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E19" sqref="E17:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
@@ -800,255 +855,313 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="10" t="s">
+      <c r="D2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="10" t="s">
+      <c r="F2" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="10" t="s">
+      <c r="H2" s="8"/>
+      <c r="I2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="11"/>
-      <c r="L2" s="3" t="s">
+      <c r="J2" s="8"/>
+      <c r="L2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="7" t="s">
         <v>58</v>
       </c>
+      <c r="N2" s="11" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="10" t="s">
+      <c r="B3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="10" t="s">
+      <c r="F3" s="8"/>
+      <c r="G3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="10" t="s">
+      <c r="H3" s="8"/>
+      <c r="I3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="11"/>
-      <c r="L3" s="3" t="s">
+      <c r="J3" s="8"/>
+      <c r="L3" s="7" t="s">
         <v>14</v>
       </c>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="10" t="s">
+      <c r="F4" s="8"/>
+      <c r="G4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="10" t="s">
+      <c r="H4" s="8"/>
+      <c r="I4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="11"/>
-      <c r="L4" s="3" t="s">
+      <c r="J4" s="8"/>
+      <c r="L4" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="13"/>
+      <c r="E5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="10" t="s">
+      <c r="F5" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="16" t="s">
+      <c r="H5" s="8"/>
+      <c r="I5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="L5" s="21" t="s">
+      <c r="J5" s="8"/>
+      <c r="L5" s="9" t="s">
         <v>18</v>
       </c>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="10" t="s">
+      <c r="D6" s="13"/>
+      <c r="E6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="10" t="s">
+      <c r="F6" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="16" t="s">
+      <c r="H6" s="8"/>
+      <c r="I6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="11"/>
-      <c r="L6" s="3" t="s">
+      <c r="J6" s="8"/>
+      <c r="L6" s="7" t="s">
         <v>41</v>
       </c>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="10" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="10" t="s">
+      <c r="D7" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="11"/>
-      <c r="L7" s="3" t="s">
+      <c r="F7" s="13"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="L7" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="10" t="s">
+      <c r="B8" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="10" t="s">
+      <c r="D8" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="11"/>
+      <c r="F8" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="10" t="s">
+      <c r="B9" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="10" t="s">
+      <c r="D9" s="13"/>
+      <c r="E9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="11"/>
+      <c r="F9" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="11"/>
+      <c r="B10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="11"/>
+      <c r="B11" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
       <c r="L11" s="6" t="s">
         <v>10</v>
       </c>
@@ -1066,61 +1179,72 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="11"/>
-      <c r="L12" s="3" t="s">
+      <c r="B12" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="L12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="M12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="N12" s="3" t="s">
+      <c r="N12" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="O12" s="3" t="s">
+      <c r="O12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="P12" s="3" t="s">
+      <c r="P12" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="11"/>
+      <c r="B13" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="11"/>
+      <c r="B14" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
       <c r="L14" s="6" t="s">
         <v>59</v>
       </c>
@@ -1138,35 +1262,47 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="13"/>
-      <c r="L15" s="21" t="s">
+      <c r="B15" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="L15" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="M15" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="N15" s="3" t="s">
+      <c r="N15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="O15" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="P15" s="3" t="s">
+      <c r="P15" s="7" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+    </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E17" s="12" t="s">
+        <v>90</v>
+      </c>
       <c r="L17" s="6" t="s">
         <v>13</v>
       </c>
@@ -1179,36 +1315,37 @@
       <c r="O17" s="6" t="s">
         <v>36</v>
       </c>
+      <c r="P17" s="8"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L18" s="3" t="s">
+      <c r="E18" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="L18" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="M18" s="3" t="s">
+      <c r="M18" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="N18" s="3" t="s">
+      <c r="N18" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="O18" s="3" t="s">
+      <c r="O18" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="P18" s="8"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" t="s">
-        <v>66</v>
-      </c>
+      <c r="E19" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E20" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" t="s">
-        <v>68</v>
-      </c>
       <c r="L20" s="6" t="s">
         <v>31</v>
       </c>
@@ -1218,52 +1355,71 @@
       <c r="N20" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G21" t="s">
-        <v>70</v>
-      </c>
-      <c r="L21" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L21" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="M21" s="3" t="s">
+      <c r="M21" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N21" s="3" t="s">
+      <c r="N21" s="7" t="s">
         <v>38</v>
       </c>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>70</v>
-      </c>
-      <c r="F22" t="s">
+        <v>64</v>
+      </c>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L24" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O24" s="10" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L24" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="M24" s="20" t="s">
+      <c r="P24" s="8"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L25" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M25" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="N24" s="20" t="s">
+      <c r="N25" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L25" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="M25" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="N25" s="17" t="s">
-        <v>0</v>
-      </c>
+      <c r="O25" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="P25" s="8"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -1272,11 +1428,13 @@
       <c r="B26" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="L26" s="17" t="s">
+      <c r="L26" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -1285,11 +1443,13 @@
       <c r="B27" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L27" s="17" t="s">
+      <c r="L27" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">

</xml_diff>

<commit_message>
docx and xlsx update
</commit_message>
<xml_diff>
--- a/New Language/Syntacticcally replaceable.xlsx
+++ b/New Language/Syntacticcally replaceable.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyGit\Front-End-Compiler-Project\New Language\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\omer\myGitHub\Front-End-Compiler-Project\New Language\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054C98D8-AB40-442C-85F0-B84564A67ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="353"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="353" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="128">
   <si>
     <t>abstract</t>
   </si>
@@ -254,9 +255,6 @@
     <t>point</t>
   </si>
   <si>
-    <t>dynamic (int/float)</t>
-  </si>
-  <si>
     <t>val</t>
   </si>
   <si>
@@ -408,12 +406,15 @@
   </si>
   <si>
     <t>@comment/@#multi-line comment#@</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dynamic </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -884,11 +885,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -912,12 +913,12 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -927,31 +928,31 @@
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>60</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>60</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>60</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>60</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>60</v>
@@ -963,34 +964,34 @@
         <v>57</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q5" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="R5" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="R5" s="6" t="s">
-        <v>98</v>
-      </c>
       <c r="S5" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U5" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="V5" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="W5" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="W5" s="6" t="s">
-        <v>108</v>
-      </c>
       <c r="X5" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y5" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="Y5" s="6" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1016,13 +1017,13 @@
         <v>21</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>31</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>29</v>
@@ -1031,34 +1032,34 @@
         <v>53</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Q6" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T6" s="7" t="s">
         <v>45</v>
       </c>
       <c r="U6" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="V6" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="V6" s="7" t="s">
-        <v>106</v>
-      </c>
       <c r="W6" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X6" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y6" s="7" t="s">
         <v>121</v>
-      </c>
-      <c r="Y6" s="7" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1082,35 +1083,35 @@
         <v>11</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>27</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="N7" s="4"/>
       <c r="P7" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q7" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R7" s="4"/>
       <c r="S7" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
       <c r="W7" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
@@ -1138,7 +1139,7 @@
         <v>16</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>38</v>
@@ -1151,18 +1152,18 @@
       </c>
       <c r="N8" s="4"/>
       <c r="P8" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
       <c r="T8" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
       <c r="W8" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
@@ -1188,18 +1189,20 @@
         <v>35</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="9"/>
+      <c r="J9" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="M9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="N9" s="4"/>
       <c r="P9" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
@@ -1208,7 +1211,7 @@
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
       <c r="W9" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
@@ -1228,20 +1231,22 @@
         <v>33</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="9"/>
+      <c r="J10" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="M10" s="3" t="s">
         <v>41</v>
       </c>
       <c r="N10" s="4"/>
       <c r="P10" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
@@ -1304,7 +1309,7 @@
         <v>12</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -1326,7 +1331,7 @@
         <v>43</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -1341,10 +1346,10 @@
         <v>5</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>3</v>
@@ -1368,7 +1373,7 @@
         <v>64</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -1400,10 +1405,10 @@
         <v>72</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -1453,7 +1458,7 @@
         <v>36</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1484,7 +1489,7 @@
         <v>55</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1534,7 +1539,7 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>60</v>
@@ -1555,10 +1560,10 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
@@ -1690,7 +1695,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>20</v>
@@ -1699,12 +1704,12 @@
         <v>30</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>24</v>
@@ -1718,7 +1723,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>6</v>
@@ -1730,7 +1735,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
valid word list checkpoint
</commit_message>
<xml_diff>
--- a/New Language/Syntacticcally replaceable.xlsx
+++ b/New Language/Syntacticcally replaceable.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\omer\myGitHub\Front-End-Compiler-Project\New Language\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects_collab\Front-End-Compiler-Project\New Language\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86552BF8-1F80-4F4B-B552-36E532BBE4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="353" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="353"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="133">
   <si>
     <t>abstract</t>
   </si>
@@ -270,9 +269,6 @@
     <t>Self</t>
   </si>
   <si>
-    <t>Const</t>
-  </si>
-  <si>
     <t>Java</t>
   </si>
   <si>
@@ -415,13 +411,25 @@
   </si>
   <si>
     <t>@comment/@@multi-line comment@@</t>
+  </si>
+  <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>const</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raise </t>
+  </si>
+  <si>
+    <t>raises</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,8 +478,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -501,6 +516,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -569,15 +590,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
@@ -624,8 +646,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="6" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="6" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
+    <cellStyle name="60% - Accent5" xfId="6" builtinId="48"/>
     <cellStyle name="Bad" xfId="5" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Input" xfId="3" builtinId="20"/>
@@ -908,14 +933,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
@@ -934,48 +959,48 @@
     <col min="23" max="23" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>60</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>60</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>60</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>60</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>60</v>
@@ -987,37 +1012,37 @@
         <v>57</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q5" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="R5" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="R5" s="6" t="s">
-        <v>97</v>
-      </c>
       <c r="S5" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="U5" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="V5" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="W5" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="W5" s="6" t="s">
-        <v>107</v>
-      </c>
       <c r="X5" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y5" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="Y5" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25">
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1046,7 +1071,7 @@
         <v>31</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>29</v>
@@ -1055,37 +1080,37 @@
         <v>53</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q6" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T6" s="7" t="s">
         <v>45</v>
       </c>
       <c r="U6" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="V6" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="V6" s="7" t="s">
-        <v>105</v>
-      </c>
       <c r="W6" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X6" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y6" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="Y6" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25">
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -1106,40 +1131,40 @@
         <v>11</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>27</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="N7" s="4"/>
       <c r="P7" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Q7" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R7" s="4"/>
       <c r="S7" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
       <c r="W7" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>44</v>
       </c>
@@ -1156,13 +1181,13 @@
         <v>0</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>38</v>
@@ -1175,23 +1200,23 @@
       </c>
       <c r="N8" s="4"/>
       <c r="P8" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
       <c r="T8" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
       <c r="W8" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -1205,7 +1230,7 @@
       <c r="E9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="23" t="s">
         <v>65</v>
       </c>
       <c r="G9" s="9" t="s">
@@ -1218,14 +1243,14 @@
         <v>17</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>17</v>
+        <v>131</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="N9" s="4"/>
       <c r="P9" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
@@ -1234,12 +1259,12 @@
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
       <c r="W9" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
@@ -1254,7 +1279,7 @@
         <v>33</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -1262,14 +1287,14 @@
         <v>22</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>22</v>
+        <v>132</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>41</v>
       </c>
       <c r="N10" s="4"/>
       <c r="P10" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
@@ -1281,7 +1306,7 @@
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>54</v>
       </c>
@@ -1315,7 +1340,7 @@
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
@@ -1339,7 +1364,7 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1361,7 +1386,7 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -1369,7 +1394,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>76</v>
@@ -1385,7 +1410,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
@@ -1395,12 +1420,12 @@
       <c r="C15" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="16" t="s">
-        <v>129</v>
+      <c r="D15" s="22" t="s">
+        <v>128</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -1422,10 +1447,10 @@
         <v>2</v>
       </c>
       <c r="R15" s="20" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
@@ -1433,10 +1458,10 @@
         <v>72</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" s="23" t="s">
         <v>124</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>125</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -1460,10 +1485,10 @@
         <v>2</v>
       </c>
       <c r="R16" s="21" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>25</v>
       </c>
@@ -1484,7 +1509,7 @@
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>36</v>
       </c>
@@ -1515,7 +1540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>55</v>
       </c>
@@ -1546,14 +1571,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M21" s="2" t="s">
         <v>13</v>
       </c>
@@ -1568,9 +1593,9 @@
       </c>
       <c r="Q21" s="4"/>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>60</v>
@@ -1589,12 +1614,12 @@
       </c>
       <c r="Q22" s="4"/>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
@@ -1602,7 +1627,7 @@
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M24" s="2" t="s">
         <v>31</v>
       </c>
@@ -1615,7 +1640,7 @@
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
         <v>59</v>
       </c>
@@ -1631,7 +1656,7 @@
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
         <v>59</v>
       </c>
@@ -1641,14 +1666,14 @@
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M28" s="6" t="s">
         <v>58</v>
       </c>
@@ -1663,7 +1688,7 @@
       </c>
       <c r="Q28" s="4"/>
     </row>
-    <row r="29" spans="1:17" ht="27">
+    <row r="29" spans="1:17" ht="28.5" x14ac:dyDescent="0.25">
       <c r="M29" s="3" t="s">
         <v>21</v>
       </c>
@@ -1678,7 +1703,7 @@
       </c>
       <c r="Q29" s="4"/>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>45</v>
       </c>
@@ -1693,7 +1718,7 @@
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
     </row>
-    <row r="31" spans="1:17" ht="27">
+    <row r="31" spans="1:17" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>47</v>
       </c>
@@ -1708,7 +1733,7 @@
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>49</v>
       </c>
@@ -1716,7 +1741,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>51</v>
       </c>
@@ -1724,9 +1749,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>20</v>
@@ -1735,12 +1760,12 @@
         <v>30</v>
       </c>
       <c r="D36" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="5" t="s">
-        <v>114</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>24</v>
@@ -1752,9 +1777,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>6</v>
@@ -1764,9 +1789,9 @@
       </c>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>42</v>

</xml_diff>